<commit_message>
Update query array in main.py for improved evaluation coverage
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2fec667f7c86ea8/Important/Capstone/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_150DD5559A7EC00F62355476585DCE3A8743B540" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{077B88D6-3332-4021-806A-D4FEF3DBDA4C}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_173585339E4AE20E62355476585DCE3A87423CA6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CA784EC-170A-4511-9CF8-2604D87867FE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>id</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>better_answer</t>
+  </si>
+  <si>
+    <t>advanced_answer</t>
+  </si>
+  <si>
+    <t>better_advanced_answer</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.22.4?</t>
   </si>
   <si>
     <t>To implement Clause B.22.4, which requires your organization to define and apply a process for redundancy on systems to ensure cyber resilience, follow these straightforward steps:
@@ -127,6 +136,9 @@
 ### 11. **Compliance and Standards:**
    - Ensure that your redundancy processes align with relevant industry standards and regulations (such as NIST, ISO 27001, etc.) to maintain compliance and bolster the organization’s cybersecurity posture.
 By following these steps and creating a robust redundancy process, you can significantly enhance the cyber resilience of your organization’s systems, thereby ensuring continuity and minimizing risks associated with system failures.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.22.5?</t>
   </si>
   <si>
     <t>To implement Clause B.22.5, which requires establishing and implementing business continuity and disaster recovery (BC/DR) policies, including roles, responsibilities, and guidelines with defined Recovery Time Objectives (RTO) and Recovery Point Objectives (RPO), follow these detailed steps:
@@ -217,6 +229,9 @@
 Implementing a BC/DR policy is an ongoing process that requires commitment, regular updates, and involvement from the entire organization. By following the steps above, you can create a robust framework that allows for effective business resumption following a disaster while meeting the specific requirements regarding system criticality, roles, responsibilities, and recovery objectives.</t>
   </si>
   <si>
+    <t>How do I implement clause B.22.6?</t>
+  </si>
+  <si>
     <t>To implement Clause B.22.6, which requires establishing and implementing a business continuity and disaster recovery (BC/DR) plan that can respond to common business disruption scenarios, including those caused by cybersecurity incidents, follow these structured steps:
 ### Step 1: Understand the Clause
 - **Business Continuity and Disaster Recovery Plan (BC/DR Plan)**: A documented strategy that outlines how your organization will continue operating during and after a disruption, especially those resulting from cyber incidents.
@@ -292,6 +307,9 @@
 By following these steps, you can develop a robust Business Continuity/Disaster Recovery plan that enhances your organization's cyber resiliency and enables effective responses to common business disruptions, including those caused by cybersecurity incidents.</t>
   </si>
   <si>
+    <t>How do I implement clause B.22.7?</t>
+  </si>
+  <si>
     <t>To implement Clause B.22.7, which requires performing regular reviews of your business continuity and disaster recovery (BC/DR) plan at least once a year to ensure it remains up-to-date, follow these simple steps:
 ### Step 1: Establish a Review Schedule
 1. **Set an Annual Review Date**: Choose a specific date each year when your organization will review the BC/DR plan. For example, you could set this for the start of the fiscal year or at the end of a significant operational period.
@@ -353,6 +371,9 @@
 ### 10. Continuous Improvement
 - **Set Up a Feedback Loop**: Encourage continuous feedback on the BC/DR plan throughout the year, not just during the annual review. This can help in making adjustments as needed.
 By following these steps, you can effectively implement a regular review process for your Business Continuity/Disaster Recovery plan, ensuring that it remains current and effective in the face of evolving risks.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.18.3?</t>
   </si>
   <si>
     <t>To implement Clause B.18.3 regarding establishing a vulnerability assessment plan, here’s a step-by-step guide tailored for you as a beginner:
@@ -441,6 +462,9 @@
 By following these steps, your organization can establish a robust Vulnerability Assessment Plan that effectively identifies, assesses, and mitigates vulnerabilities in its systems, ultimately enhancing its overall security posture.</t>
   </si>
   <si>
+    <t>How do I implement clause B.22.9?</t>
+  </si>
+  <si>
     <t>To implement Clause B.22.9, which requires your organization to monitor Recovery Time Objectives (RTO) and Recovery Point Objectives (RPO) during business continuity and disaster recovery (BC/DR) processes, and report these findings to senior management, follow these structured steps:
 ### Step 1: Understand RTO and RPO
 1. **Define RTO and RPO**: Ensure everyone involved understands what RTO and RPO mean:
@@ -521,6 +545,9 @@
 By following these steps, your organization can effectively monitor compliance with RTO and RPO, enabling you to minimize downtime and data loss while maintaining transparency with senior leadership.</t>
   </si>
   <si>
+    <t>How do I implement clause B.22.10?</t>
+  </si>
+  <si>
     <t>To implement Clause B.22.10, which requires your organization to perform coordinated business continuity and disaster recovery (BC/DR) exercises with third parties, follow these structured steps:
 ### Step 1: Identify Third Parties
 1. **List Key Third Parties**: Identify all third-party suppliers, partners, and vendors that are critical to your business operations and whose services may impact your BC/DR plans.
@@ -593,6 +620,9 @@
 By implementing these steps, you will create an effective and ongoing program for business continuity and disaster recovery exercises that involve third parties. This will help ensure better preparedness for actual incidents and foster a culture of resilience within your organization and among its partners.</t>
   </si>
   <si>
+    <t>How do I implement clause B.18.6?</t>
+  </si>
+  <si>
     <t>To implement clause B.18.6, which requires your organization to establish and implement policies and procedures for conducting cybersecurity vulnerability assessments, follow these steps:
 ### Step-by-Step Implementation
 1. **Understand the Purpose**:
@@ -655,6 +685,9 @@
 ### Example Policy Statement
 "The organization shall conduct comprehensive vulnerability assessments at least quarterly or upon significant changes to its IT environment. All identified vulnerabilities will be categorized by severity, documented, and remediated according to established timelines based on their risk profile. Continuous improvement of the assessment process will be pursued through regular reviews, staff training, and updates to the policy."
 By following these steps, your organization can establish a robust vulnerability assessment policy and procedure that effectively reduces risk and enhances the overall security posture.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.18.7?</t>
   </si>
   <si>
     <t>To implement clause B.18.7, which requires your organization to establish and implement measures to track, review, evaluate, and address vulnerabilities uncovered during assessments, follow these steps:
@@ -726,6 +759,9 @@
    - **Align with Incident Response**: Ensure that vulnerability management is integrated with the overall incident response plan to handle incidents arising from unremediated vulnerabilities.
 ### Conclusion
 By implementing these steps, your organization can effectively track and remediate identified vulnerabilities, ensuring that they are addressed according to severity and minimizing the risk of exploitation. Maintain documentation and adjust processes as necessary to align with evolving threats and organizational goals.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.18.8?</t>
   </si>
   <si>
     <t>To implement clause B.18.8, which requires your organization to establish and implement a penetration test plan, follow these steps:
@@ -816,6 +852,9 @@
 By following these steps, you can establish a comprehensive penetration testing plan that aligns with organizational priorities, enhances security posture, and ensures safety and compliance during the testing process.</t>
   </si>
   <si>
+    <t>How do I implement clause B.18.10?</t>
+  </si>
+  <si>
     <t>To implement clause B.18.10, which requires your organization to establish and implement metrics and thresholds for tracking vulnerabilities, follow these steps:
 ### Step-by-Step Implementation
 1. **Understand the Objective**:
@@ -900,6 +939,9 @@
 By following these steps, your organization will be better positioned to monitor, track, and remediate vulnerabilities effectively. This structured approach not only enhances visibility on vulnerabilities but also fosters a culture of security awareness within the organization.</t>
   </si>
   <si>
+    <t>How do I implement clause B.18.11?</t>
+  </si>
+  <si>
     <t>To implement clause B.18.11, which requires your organization to regularly report vulnerability assessment results to the Board and/or senior management, follow these steps:
 ### Step-by-Step Implementation
 1. **Understand the Importance of Reporting**:
@@ -977,6 +1019,9 @@
 By establishing a clear framework for reporting vulnerability assessment results, your organization can ensure that the Board and senior management are informed about potential risks. This enables more informed decision-making and enhances the organization's overall security posture.</t>
   </si>
   <si>
+    <t>How do I implement clause B.19.2?</t>
+  </si>
+  <si>
     <t>To implement clause B.19.2 regarding physical/environmental security, follow these clear steps:
 ### Step-by-Step Guide to Implementing Clause B.19.2
 1. **Identify Physical/Environmental Risks**:
@@ -1030,6 +1075,9 @@
 - **Policy Documentation**: Create and maintain detailed documentation of all policies, procedures, and configurations for the systems in place.
 - **Audit Trails**: Keep records of audits and system checks performed, providing a track record of compliance and operational readiness.
 By following these steps, your organization can establish effective detective controls that not only identify physical and environmental risks but also ensure timely alerts and responses to threats. This proactive approach enhances the resilience and safety of your operations.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.19.3?</t>
   </si>
   <si>
     <t>To implement clause B.19.3, which focuses on protecting your physical assets against internal and external threats, follow these straightforward steps:
@@ -1095,6 +1143,9 @@
    - **Continuous Improvement**: Regularly review policies and procedures to ensure they remain effective and relevant as new threats emerge or as the organization evolves.
 ### Conclusion
 By systematically assessing risks, implementing physical measures, training employees, and regularly reviewing security policies, your organization can effectively safeguard its physical assets against both internal and external threats. Ensure that all measures are documented and communicated to all relevant stakeholders for maximum effectiveness.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.19.5?</t>
   </si>
   <si>
     <t>To implement clause B.19.5, which requires a process for registering and authorizing visitors before they access your premises, follow these clear steps:
@@ -1174,6 +1225,9 @@
 By following these steps, you can ensure that visitors are adequately registered and authorized before accessing your organization's premises, thereby enhancing security and safety.</t>
   </si>
   <si>
+    <t>How do I implement clause B.19.6?</t>
+  </si>
+  <si>
     <t>To implement clause B.19.6, which focuses on establishing a 24/7 monitoring process for your premises, follow these clear steps:
 ### Step-by-Step Guide to Implementing Clause B.19.6
 1. **Assess Your Monitoring Needs**:
@@ -1237,6 +1291,9 @@
 - **Annual Review**: Regularly review the security policy and monitoring processes to adapt to new threats, technologies, or changes in organizational needs.
 ### Conclusion
 By following these steps systematically, your organization can implement a robust monitoring process using CCTV and other security measures to ensure the safety and security of its premises around the clock. This not only helps deter criminal activity but also fosters a safer environment for employees and customers.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.19.7?</t>
   </si>
   <si>
     <t>To implement clause B.19.7, which involves securely storing and transporting physical media containing business-critical data, follow these structured steps:
@@ -1312,6 +1369,9 @@
 By following these steps, organizations can create a comprehensive physical media handling process that secures the storage and transport of business-critical data, ensuring that confidential and sensitive information is adequately protected.</t>
   </si>
   <si>
+    <t>How do I implement clause B.19.9?</t>
+  </si>
+  <si>
     <t>To implement clause B.19.9, which involves defining and allocating roles and responsibilities for detecting, mitigating, and responding to physical/environmental risks, follow these organized steps:
 ### Step-by-Step Guide to Implementing Clause B.19.9
 1. **Identify Physical/Environmental Risks**:
@@ -1381,6 +1441,9 @@
 | Safety Coordinator | Lead safety training sessions, ensure compliance with safety regulations, and manage incident response protocols. | 
 | Employees | Report potential risks, participate in training programs, and follow safety procedures. | 
 Implementing the clause effectively requires ongoing commitment and engagement from all levels of the organization, ensuring that everyone understands their role in mitigating risks and responding to emergencies.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.19.10?</t>
   </si>
   <si>
     <t>To implement clause B.19.10, which requires the establishment of policies and procedures for reviewing physical security measures and assets, follow these organized steps:
@@ -1457,6 +1520,9 @@
 By following these steps and maintaining a continuous improvement mindset, you can effectively implement the clause regarding the review of physical and environmental security measures in your organization.</t>
   </si>
   <si>
+    <t>How do I implement clause B.20.5?</t>
+  </si>
+  <si>
     <t>To implement Clause B.20.5, which requires secure configuration of both wired and wireless networks, follow these straightforward steps:
 ### Step-by-Step Implementation of Clause B.20.5
 1. **Define Network Security Policies**:
@@ -1527,6 +1593,33 @@
 Implementing a secure network configuration process is an ongoing effort that requires careful planning, activities, and regular reviews. By following these steps, you can enhance the security of both wired and wireless networks to minimize data breaches and unauthorized access.</t>
   </si>
   <si>
+    <t>To implement Clause B.20.5, which focuses on the secure configuration of both wired and wireless networks, follow these advanced steps:
+1. **Define Network Security Policies**:
+   - Establish comprehensive network security policies that outline requirements for both wired and wireless network configurations. Ensure these policies include guidelines for secure authentication, encryption, and the disabling of Wi-Fi Protected Setup (WPS).
+2. **Secure Wired Network Configuration**:
+   - **Authentication**: Implement strong authentication mechanisms for all devices connected to the wired network, such as 802.1X port-based network access control.
+   - **Encryption**: Utilize protocols like IPsec to encrypt data in transit across your wired network, ensuring confidentiality and integrity.
+   - **Device Hardening**: Regularly update and patch network devices (routers, switches) to mitigate vulnerabilities.
+3. **Secure Wireless Network Configuration**:
+   - **Authentication**: Use WPA3 for secure wireless authentication. If WPA3 is not available, ensure WPA2 is configured with a strong pre-shared key.
+   - **Encryption**: Ensure that encryption protocols such as AES (Advanced Encryption Standard) are enabled for all wireless communications.
+   - **Disable WPS**: Disable Wi-Fi Protected Setup (WPS) on all wireless routers and access points to eliminate vulnerabilities associated with easy connections.
+   - **SSID Management**: Use non-identifiable SSIDs that do not reveal the network type or organization. Regularly rotate SSIDs if necessary.
+4. **Network Segmentation**:
+   - Implement network segmentation to isolate sensitive systems and data. This can be achieved using VLANs for wired networks and separate SSIDs for wireless networks, limiting access to sensitive data.
+5. **Implement VPNs for Remote Access**:
+   - For secure remote access to the network, implement Virtual Private Networks (VPNs). Use strong encryption protocols (e.g., OpenVPN or IPsec) to secure communications between remote users and the organization’s network.
+6. **Regular Audits and Testing**:
+   - Schedule regular audits of network configurations and conduct penetration testing to identify and rectify vulnerabilities. Ensure compliance with the established security policies.
+7. **Documentation and Training**:
+   - Document all security configurations and policies. Provide training for IT staff on best practices for maintaining network security and handling security incidents.
+By following these steps, you can effectively implement Clause B.20.5 and ensure that both wired and wireless networks are configured securely.
+What types of network devices and protocols do you currently use in your infrastructure? This information will help tailor further recommendations specific to your environment.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.19.12?</t>
+  </si>
+  <si>
     <t>To implement clause B.19.12, which requires establishing a process to review and improve physical and environmental security measures, follow these organized steps:
 ### Step-by-Step Guide to Implementing Clause B.19.12
 1. **Develop a Review Policy**:
@@ -1593,6 +1686,9 @@
    - **External Assessment**: Consider engaging third parties for an external review or audit of your security measures.
 ### Conclusion
 By following these steps, your organization can establish an effective process for reviewing and improving physical and environmental security measures, thereby ensuring their ongoing relevance and effectiveness against evolving threats.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.20.2?</t>
   </si>
   <si>
     <t>To implement Clause B.20.2, which focuses on configuring and implementing access control to your network, you can follow these straightforward steps:
@@ -1663,6 +1759,28 @@
 ### 10. **Incident Response Plan**
    - **Prepare an Incident Response Plan**: Establish a detailed plan for responding to security incidents, including how to handle unauthorized access attempts.
 By following these steps, an organization can effectively implement access control to its network, helping to ensure compliance with its security policies and reduce the risk of unauthorized access. Regular assessments and updates to the access control mechanisms are essential to adapting to evolving threats and organizational changes.</t>
+  </si>
+  <si>
+    <t>To implement Clause B.20.2, which requires configuring and implementing access control (e.g., whitelisting, blacklisting) to your network, follow these high-level steps:
+1. **Identify Access Control Requirements**:
+   - Assess the network architecture to understand where access control is needed (e.g., subnets, specific servers, applications).
+2. **Choose Access Control Mechanisms**:
+   - **Network Access Control Lists (ACLs)**: Create and configure ACLs for your Virtual Private Cloud (VPC) to control inbound and outbound traffic. These ACLs can be set to allow or deny traffic based on IP addresses, protocols, and ports.
+   - **Security Groups**: Utilize security groups as virtual firewalls for your resources. Define rules that specify which traffic is allowed to and from your resources based on applications and services.
+3. **Implement Whitelisting and Blacklisting**:
+   - **Whitelisting**: Identify and allow only trusted IP addresses or devices to access your network resources. This is crucial for sensitive applications.
+   - **Blacklisting**: Identify and deny access to known malicious IP addresses or devices. Regularly update your blacklist based on threat intelligence.
+4. **Use Advanced Security Solutions**:
+   - **AWS Network Firewall**: For an additional layer of security, consider deploying AWS Network Firewall. This service provides stateful traffic inspection and intrusion detection/prevention capabilities tailored for your VPC.
+5. **Continuous Monitoring and Updates**:
+   - Implement monitoring solutions to log access attempts and alerts for unauthorized access. Regularly review and update your access control policies and configurations to adapt to new threats.
+6. **Documentation and Policy Enforcement**:
+   - Document your access control policies and ensure they are enforced across the organization. Train staff on the importance of these controls and how to maintain them.
+By following these steps, you can ensure that unauthorized users or devices are kept out of your network, thus adhering to the requirements of Clause B.20.2.
+Do you currently use any specific cloud infrastructure or on-premises technologies for your network? This will help in providing more tailored recommendations.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.20.3?</t>
   </si>
   <si>
     <t>To implement Clause B.20.3, which involves establishing and using a stateful firewall over a basic packet filtering firewall, follow these simple steps:
@@ -1739,6 +1857,188 @@
 By implementing a stateful firewall effectively, you can enhance your organization’s network security by providing better context to network traffic, enabling more granular control over how packets are filtered and allowing for dynamic responses to network traffic.</t>
   </si>
   <si>
+    <t>To implement Clause B.20.3, which mandates the establishment and use of a stateful firewall over a basic packet filtering firewall, follow these advanced steps:
+1. **Assess Current Firewall Infrastructure**:
+   - Review your existing firewall setup. Determine if you are currently using a basic packet filtering firewall and identify any limitations it may have in context-aware filtering.
+2. **Select a Stateful Firewall Solution**:
+   - Choose a stateful firewall that meets your network requirements. Options include:
+     - **AWS Network Firewall**: A fully managed service that provides stateful inspection and integrates well with AWS environments.
+     - **Azure Firewall**: If you're on Azure, consider Azure Firewall, which provides stateful packet inspection with advanced threat protection.
+     - **On-Premises Solutions**: If your infrastructure is on-premises, consider solutions like Palo Alto Networks or Fortinet that offer robust stateful inspection capabilities.
+3. **Implement Configuration**:
+   - **Define Security Rules**: Configure the stateful firewall rules to allow or deny traffic based on established policies. Ensure that rules take into account session states, allowing return traffic based on established sessions.
+   - **Integrate with Existing Infrastructure**: If using a cloud provider, integrate the stateful firewall with your existing network architecture (e.g., VPC, subnets).
+4. **Enable Logging and Monitoring**:
+   - Configure logging features on the firewall to monitor traffic patterns, detect anomalies, and respond to potential threats. Implement alerting mechanisms to notify your security team of suspicious activities.
+5. **Test the Firewall Configuration**:
+   - Conduct thorough testing of the firewall rules to ensure they are correctly filtering traffic as intended. Use penetration testing tools to validate the effectiveness of the stateful firewall.
+6. **Regular Review and Maintenance**:
+   - Establish a routine for reviewing firewall rules and configurations. Update them as necessary to adapt to evolving threats and changes in network architecture.
+7. **Documentation and Training**:
+   - Document the firewall configuration, policies, and procedures. Provide training for your IT and security teams on the features and management of the stateful firewall.
+By following these steps, you can effectively implement Clause B.20.3 and enhance your network security posture through context-aware filtering.
+What type of firewall do you currently have in place, and what specific security challenges are you facing? This will help tailor recommendations further.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.20.8?</t>
+  </si>
+  <si>
+    <t>To implement Clause B.20.8, which requires defining and allocating roles and responsibilities for managing and monitoring network security, follow these steps:
+### Step-by-Step Implementation of Clause B.20.8
+1. **Identify Key Roles**:
+   - Determine the critical roles necessary for effective network security management. Common roles may include:
+     - **Network Security Officer**: Responsible for overall security strategy and compliance.
+     - **Network Administrator**: Manages day-to-day operations of the network, including configuration and monitoring.
+     - **Security Analyst**: Monitors network traffic and analyzes security incidents.
+     - **Incident Response Team Member**: Responds to security breaches or incidents.
+2. **Define Responsibilities**:
+   - Clearly outline the responsibilities associated with each role. For example:
+     - **Network Security Officer**: Develops security policies, oversees audits, and ensures compliance with regulations.
+     - **Network Administrator**: Configures firewalls, applies updates, and manages user access.
+     - **Security Analyst**: Conducts vulnerability assessments and reports on security incidents.
+3. **Create a Role Responsibility Matrix**:
+   - Develop a document that lists all roles alongside their specific responsibilities. This can serve as a reference for employees and help clarify tasks.
+   - For example, use a table format where each row represents a role, and columns indicate specific tasks or responsibilities.
+4. **Assign Roles to Employees**:
+   - Allocate these defined roles to specific employees based on their skills, expertise, and job functions. Ensure that everyone understands their assigned responsibilities.
+5. **Provide Training and Resources**:
+   - Offer training to ensure employees understand their roles and the importance of their tasks in maintaining network security. This could include:
+     - Workshops on security best practices.
+     - Regular updates on emerging threats and security technologies.
+6. **Establish Communication Channels**:
+   - Create clear communication pathways for reporting security issues and discussing security concerns. This could involve regular team meetings or a dedicated communication platform.
+7. **Regularly Review and Update Roles**:
+   - Periodically review the roles and responsibilities to ensure they remain relevant as your organization grows or changes. Update them based on new security requirements or technological advancements.
+8. **Document Everything**:
+   - Keep records of the roles, responsibilities, and any changes made. This documentation will be important for audits and compliance checks.
+### Example:
+If you have an IT department, you might designate one employee as the Network Security Officer who is responsible for policy development, another as a Security Analyst tasked with monitoring network activity, and a third as a Network Administrator who handles device configurations.
+### Next Steps:
+Consider creating a formal document that outlines these roles and responsibilities and sharing it with your team to ensure clarity and accountability.
+**Question for You:**
+Do you currently have a team in place, or would you need assistance in identifying and defining these roles based on your organization's structure?</t>
+  </si>
+  <si>
+    <t>Implementing a clause for "Roles and Responsibilities" in your organization’s network security framework involves several steps. Here's a structured approach to help you ensure that roles and responsibilities are well-defined, managed, and communicated:
+### 1. **Define Network Security Roles:**
+   - **Identify Key Roles:** Start by defining roles related to network security, such as:
+     - Chief Information Security Officer (CISO)
+     - Network Security Manager
+     - Cybersecurity Analyst
+     - System Administrator
+     - Incident Response Team Lead
+     - IT Support Staff
+     - End-users
+   - **Create Role Descriptions:** For each identified role, create detailed job descriptions that outline:
+     - Objectives and responsibilities
+     - Required qualifications and skills
+     - Reporting relationships
+     - Decision-making authority
+### 2. **Develop a Responsibility Matrix:**
+   - **RACI Model:** Use a Responsibility Assignment Matrix (often called a RACI matrix - Responsible, Accountable, Consulted, Informed) to clarify who does what.
+     - Responsible: Who is responsible for carrying out the task?
+     - Accountable: Who is ultimately accountable for the completion?
+     - Consulted: Who needs to be consulted before a decision is made?
+     - Informed: Who needs to be kept informed about the progress?
+### 3. **Establish Policies and Procedures:**
+   - Develop specific policies related to network security, including access controls, data protection, incident response, etc.
+   - Document standard operating procedures (SOPs) that delineate how security tasks should be performed, ensuring consistency and clarity.
+### 4. **Communicate Roles and Responsibilities:**
+   - **Training and Awareness:** Implement regular training sessions to inform employees about their specific roles and responsibilities related to network security.
+   - **Documentation Accessibility:** Make sure that the documented roles, responsibilities, policies, and procedures are easily accessible to all employees. Utilize a central repository.
+   - **Onboarding New Employees:** Integrate network security responsibilities into the onboarding process for new employees.
+### 5. **Monitor and Review:**
+   - **Performance Metrics:** Establish KPIs or metrics to monitor the effectiveness of the assigned roles. This could include response times to incidents, number of security breaches, etc.
+   - **Regular Reviews:** Periodically review the roles and responsibilities to ensure they remain relevant as technologies and business needs evolve.
+   - **Feedback Mechanism:** Create a mechanism for employees to provide feedback on their responsibilities and the clarity of their roles.
+### 6. **Compliance and Documentation:**
+   - Ensure that all defined roles and responsibilities are compliant with relevant regulations and standards (e.g., ISO 27001, NIST).
+   - Maintain proper documentation to demonstrate oversight and management of network security roles and responsibilities, which can help during audits.
+### 7. **Continuous Improvement:**
+   - Foster a culture of continuous improvement where employees are encouraged to suggest changes based on new threats, technology adoption, or organizational changes.
+   - Regularly update training materials and documentation based on the feedback and findings from security incidents.
+### Conclusion
+Implementing a robust framework for roles and responsibilities related to network security will ensure clarity for employees, help in effective management, and enhance the overall security posture of your organization. This approach also helps in creating accountability and reinforces the importance of each individual’s role in the larger network security strategy.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.20.9?</t>
+  </si>
+  <si>
+    <t>To implement Clause B.20.9, which involves establishing and implementing network intrusion detection to monitor and detect malicious network traffic, follow these steps:
+### Step-by-Step Implementation of Clause B.20.9
+1. **Choose an Intrusion Detection Solution**:
+   - Decide on a network intrusion detection system (NIDS) or service that fits your infrastructure. If you are using cloud services like AWS, consider using:
+     - **AWS Network Firewall**: A managed service that provides intrusion detection and prevention.
+     - **AWS WAF (Web Application Firewall)**: This can help monitor web traffic specifically for your applications.
+2. **Configure Network Intrusion Detection**:
+   - **For AWS Network Firewall**:
+     - Access the AWS Management Console.
+     - Navigate to the **Network Firewall** section and create a new firewall.
+     - Set up rules to inspect network traffic, including defining known bad domains, and configuring deep packet inspection.
+   - **For AWS WAF**:
+     - Go to the **WAF** section in the AWS Console.
+     - Create a Web ACL (Access Control List) to define conditions for monitoring web requests. This can include IP address filtering, request rate limiting, or specific request attributes.
+3. **Set Up Alerts and Notifications**:
+   - Configure the system to send alerts when it detects suspicious activity or potential intrusions. This can involve setting up email notifications or integrating with a security information and event management (SIEM) system.
+4. **Regularly Review Logs and Reports**:
+   - Periodically review the logs generated by the intrusion detection system. Look for patterns or repeated attempts at unauthorized access.
+   - Use the insights from these logs to adjust your security posture and improve your detection capabilities.
+5. **Establish an Incident Response Plan**:
+   - Develop a plan for how your organization will respond to detected intrusions. This plan should include:
+     - Procedures for containing the threat.
+     - Communication strategies for informing stakeholders.
+     - Steps for investigating the incident and preventing future occurrences.
+6. **Conduct Regular Testing and Updates**:
+   - Regularly test your intrusion detection system to ensure it functions correctly. Simulate attacks to see if the system detects them.
+   - Keep the system updated with the latest threat intelligence and signatures to improve detection capabilities.
+7. **Train Staff on Intrusion Detection**:
+   - Provide training for your team on how to interpret alerts from the intrusion detection system and how to respond appropriately.
+### Example:
+If you configure AWS Network Firewall, you can set rules that will automatically block traffic from known malicious IP addresses and alert your security team whenever there is an attempted intrusion.
+### Next Steps:
+Consider documenting your intrusion detection policies and procedures to ensure that all team members are aware of their roles in monitoring and responding to potential threats.
+**Question for You:**
+Do you currently have any existing intrusion detection systems in place, or are you starting from scratch?</t>
+  </si>
+  <si>
+    <t>Implementing a network intrusion detection system (NIDS) involves several key steps to ensure that malicious network traffic is effectively monitored, detected, and addressed. Here’s a structured approach you can follow:
+### 1. Define Objectives and Requirements
+- **Identify Goals**: Clearly define what you want to achieve with your NIDS (e.g., real-time threat detection, compliance, improved incident response).
+- **Assess Requirements**: Determine the technical and resource requirements based on the network architecture, size, and critical assets of your organization.
+### 2. Select NIDS Solutions
+- **Choose a Technology**: Evaluate and select a network intrusion detection system that meets your needs. Options include software-based solutions (e.g., Snort, Suricata) or hardware appliances.
+- **Consider Open-Source vs. Commercial**: Decide whether to use open-source solutions, which may require more customization but can be cost-effective, or commercial systems that often come with support.
+### 3. Design Network Architecture
+- **Identify Key Areas**: Determine where to place NIDS sensors based on traffic flow, segmentation, and monitoring needs (e.g., at the perimeter, critical internal switch ports).
+- **Plan for Deployment**: Ensure that the network design accommodates the installation of NIDS, including appropriate bandwidth and security measures.
+### 4. Install and Configure NIDS
+- **Installation**: Follow the installation procedures for your chosen NIDS solution.
+- **Configuration**: Configure the system to monitor relevant network traffic, including defining rules and policies for alerting on suspicious activities. Tailor the settings to minimize false positives.
+### 5. Establish Monitoring and Alerting
+- **Set Up Alerts**: Configure alerting mechanisms so that incidents are reported to administrators or security teams in real-time.
+- **Integrate with SIEM**: Consider integrating the NIDS with a Security Information and Event Management (SIEM) system for centralized logging and advanced analysis.
+### 6. Develop Response Procedures
+- **Incident Response Plan**: Create a plan outlining how to address potential intrusions detected by the NIDS, including roles and responsibilities, investigation steps, and communication protocols.
+- **Escalation Procedures**: Define when and how to escalate incidents based on severity levels.
+### 7. Train Personnel
+- **Training Sessions**: Conduct training for your IT and security teams on how to utilize the NIDS effectively and respond to alerts.
+- **Simulated Exercises**: Regularly engage in security drills to test the effectiveness of your response procedures and the competence of your personnel.
+### 8. Continuous Monitoring and Maintenance
+- **Ongoing Monitoring**: Keep the NIDS active and continuously monitor its performance.
+- **Regular Updates**: Apply updates to the NIDS, including signature updates and system patches, to ensure it stays effective against new threats.
+- **Review and Adjust**: Periodically review policies, rules, and configurations to adapt to the changing network environment and threat landscape.
+### 9. Audit and Review
+- **Regular Audits**: Conduct regular audits of the NIDS configuration, monitoring effectiveness, and incident response performance.
+- **Reporting**: Generate reports to analyze trends, identify gaps, and support compliance requirements.
+### 10. Compliance and Documentation
+- **Document Policies and Procedures**: Ensure that all NIDS-related procedures, configurations, and policies are well documented.
+- **Compliance Check**: Make sure that your implementation aligns with relevant regulatory requirements (e.g., GDPR, PCI-DSS, HIPAA).
+By following these steps, you can effectively establish and implement a network intrusion detection system that monitors your organization's network for malicious activity, allowing you to quickly identify and address potential threats.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.20.7?</t>
+  </si>
+  <si>
     <t>To implement Clause B.20.7, which requires the establishment and implementation of security policies and procedures to harden your network architecture, devices, and access security, follow these steps:
 ### Step-by-Step Implementation of Clause B.20.7
 1. **Define Security Objectives**:
@@ -1818,154 +2118,39 @@
 By following these steps, you can establish a robust framework for network security policies and procedures that effectively harden your network architecture, device security, and access controls. It’s important to adapt these steps according to your organization’s size, industry, and specific needs.</t>
   </si>
   <si>
-    <t>To implement Clause B.20.8, which requires defining and allocating roles and responsibilities for managing and monitoring network security, follow these steps:
-### Step-by-Step Implementation of Clause B.20.8
-1. **Identify Key Roles**:
-   - Determine the critical roles necessary for effective network security management. Common roles may include:
-     - **Network Security Officer**: Responsible for overall security strategy and compliance.
-     - **Network Administrator**: Manages day-to-day operations of the network, including configuration and monitoring.
-     - **Security Analyst**: Monitors network traffic and analyzes security incidents.
-     - **Incident Response Team Member**: Responds to security breaches or incidents.
-2. **Define Responsibilities**:
-   - Clearly outline the responsibilities associated with each role. For example:
-     - **Network Security Officer**: Develops security policies, oversees audits, and ensures compliance with regulations.
-     - **Network Administrator**: Configures firewalls, applies updates, and manages user access.
-     - **Security Analyst**: Conducts vulnerability assessments and reports on security incidents.
-3. **Create a Role Responsibility Matrix**:
-   - Develop a document that lists all roles alongside their specific responsibilities. This can serve as a reference for employees and help clarify tasks.
-   - For example, use a table format where each row represents a role, and columns indicate specific tasks or responsibilities.
-4. **Assign Roles to Employees**:
-   - Allocate these defined roles to specific employees based on their skills, expertise, and job functions. Ensure that everyone understands their assigned responsibilities.
-5. **Provide Training and Resources**:
-   - Offer training to ensure employees understand their roles and the importance of their tasks in maintaining network security. This could include:
-     - Workshops on security best practices.
-     - Regular updates on emerging threats and security technologies.
-6. **Establish Communication Channels**:
-   - Create clear communication pathways for reporting security issues and discussing security concerns. This could involve regular team meetings or a dedicated communication platform.
-7. **Regularly Review and Update Roles**:
-   - Periodically review the roles and responsibilities to ensure they remain relevant as your organization grows or changes. Update them based on new security requirements or technological advancements.
-8. **Document Everything**:
-   - Keep records of the roles, responsibilities, and any changes made. This documentation will be important for audits and compliance checks.
-### Example:
-If you have an IT department, you might designate one employee as the Network Security Officer who is responsible for policy development, another as a Security Analyst tasked with monitoring network activity, and a third as a Network Administrator who handles device configurations.
-### Next Steps:
-Consider creating a formal document that outlines these roles and responsibilities and sharing it with your team to ensure clarity and accountability.
-**Question for You:**
-Do you currently have a team in place, or would you need assistance in identifying and defining these roles based on your organization's structure?</t>
-  </si>
-  <si>
-    <t>Implementing a clause for "Roles and Responsibilities" in your organization’s network security framework involves several steps. Here's a structured approach to help you ensure that roles and responsibilities are well-defined, managed, and communicated:
-### 1. **Define Network Security Roles:**
-   - **Identify Key Roles:** Start by defining roles related to network security, such as:
-     - Chief Information Security Officer (CISO)
-     - Network Security Manager
-     - Cybersecurity Analyst
-     - System Administrator
-     - Incident Response Team Lead
-     - IT Support Staff
-     - End-users
-   - **Create Role Descriptions:** For each identified role, create detailed job descriptions that outline:
-     - Objectives and responsibilities
-     - Required qualifications and skills
-     - Reporting relationships
-     - Decision-making authority
-### 2. **Develop a Responsibility Matrix:**
-   - **RACI Model:** Use a Responsibility Assignment Matrix (often called a RACI matrix - Responsible, Accountable, Consulted, Informed) to clarify who does what.
-     - Responsible: Who is responsible for carrying out the task?
-     - Accountable: Who is ultimately accountable for the completion?
-     - Consulted: Who needs to be consulted before a decision is made?
-     - Informed: Who needs to be kept informed about the progress?
-### 3. **Establish Policies and Procedures:**
-   - Develop specific policies related to network security, including access controls, data protection, incident response, etc.
-   - Document standard operating procedures (SOPs) that delineate how security tasks should be performed, ensuring consistency and clarity.
-### 4. **Communicate Roles and Responsibilities:**
-   - **Training and Awareness:** Implement regular training sessions to inform employees about their specific roles and responsibilities related to network security.
-   - **Documentation Accessibility:** Make sure that the documented roles, responsibilities, policies, and procedures are easily accessible to all employees. Utilize a central repository.
-   - **Onboarding New Employees:** Integrate network security responsibilities into the onboarding process for new employees.
-### 5. **Monitor and Review:**
-   - **Performance Metrics:** Establish KPIs or metrics to monitor the effectiveness of the assigned roles. This could include response times to incidents, number of security breaches, etc.
-   - **Regular Reviews:** Periodically review the roles and responsibilities to ensure they remain relevant as technologies and business needs evolve.
-   - **Feedback Mechanism:** Create a mechanism for employees to provide feedback on their responsibilities and the clarity of their roles.
-### 6. **Compliance and Documentation:**
-   - Ensure that all defined roles and responsibilities are compliant with relevant regulations and standards (e.g., ISO 27001, NIST).
-   - Maintain proper documentation to demonstrate oversight and management of network security roles and responsibilities, which can help during audits.
-### 7. **Continuous Improvement:**
-   - Foster a culture of continuous improvement where employees are encouraged to suggest changes based on new threats, technology adoption, or organizational changes.
-   - Regularly update training materials and documentation based on the feedback and findings from security incidents.
-### Conclusion
-Implementing a robust framework for roles and responsibilities related to network security will ensure clarity for employees, help in effective management, and enhance the overall security posture of your organization. This approach also helps in creating accountability and reinforces the importance of each individual’s role in the larger network security strategy.</t>
-  </si>
-  <si>
-    <t>To implement Clause B.20.9, which involves establishing and implementing network intrusion detection to monitor and detect malicious network traffic, follow these steps:
-### Step-by-Step Implementation of Clause B.20.9
-1. **Choose an Intrusion Detection Solution**:
-   - Decide on a network intrusion detection system (NIDS) or service that fits your infrastructure. If you are using cloud services like AWS, consider using:
-     - **AWS Network Firewall**: A managed service that provides intrusion detection and prevention.
-     - **AWS WAF (Web Application Firewall)**: This can help monitor web traffic specifically for your applications.
-2. **Configure Network Intrusion Detection**:
-   - **For AWS Network Firewall**:
-     - Access the AWS Management Console.
-     - Navigate to the **Network Firewall** section and create a new firewall.
-     - Set up rules to inspect network traffic, including defining known bad domains, and configuring deep packet inspection.
-   - **For AWS WAF**:
-     - Go to the **WAF** section in the AWS Console.
-     - Create a Web ACL (Access Control List) to define conditions for monitoring web requests. This can include IP address filtering, request rate limiting, or specific request attributes.
-3. **Set Up Alerts and Notifications**:
-   - Configure the system to send alerts when it detects suspicious activity or potential intrusions. This can involve setting up email notifications or integrating with a security information and event management (SIEM) system.
-4. **Regularly Review Logs and Reports**:
-   - Periodically review the logs generated by the intrusion detection system. Look for patterns or repeated attempts at unauthorized access.
-   - Use the insights from these logs to adjust your security posture and improve your detection capabilities.
-5. **Establish an Incident Response Plan**:
-   - Develop a plan for how your organization will respond to detected intrusions. This plan should include:
-     - Procedures for containing the threat.
-     - Communication strategies for informing stakeholders.
-     - Steps for investigating the incident and preventing future occurrences.
-6. **Conduct Regular Testing and Updates**:
-   - Regularly test your intrusion detection system to ensure it functions correctly. Simulate attacks to see if the system detects them.
-   - Keep the system updated with the latest threat intelligence and signatures to improve detection capabilities.
-7. **Train Staff on Intrusion Detection**:
-   - Provide training for your team on how to interpret alerts from the intrusion detection system and how to respond appropriately.
-### Example:
-If you configure AWS Network Firewall, you can set rules that will automatically block traffic from known malicious IP addresses and alert your security team whenever there is an attempted intrusion.
-### Next Steps:
-Consider documenting your intrusion detection policies and procedures to ensure that all team members are aware of their roles in monitoring and responding to potential threats.
-**Question for You:**
-Do you currently have any existing intrusion detection systems in place, or are you starting from scratch?</t>
-  </si>
-  <si>
-    <t>Implementing a network intrusion detection system (NIDS) involves several key steps to ensure that malicious network traffic is effectively monitored, detected, and addressed. Here’s a structured approach you can follow:
-### 1. Define Objectives and Requirements
-- **Identify Goals**: Clearly define what you want to achieve with your NIDS (e.g., real-time threat detection, compliance, improved incident response).
-- **Assess Requirements**: Determine the technical and resource requirements based on the network architecture, size, and critical assets of your organization.
-### 2. Select NIDS Solutions
-- **Choose a Technology**: Evaluate and select a network intrusion detection system that meets your needs. Options include software-based solutions (e.g., Snort, Suricata) or hardware appliances.
-- **Consider Open-Source vs. Commercial**: Decide whether to use open-source solutions, which may require more customization but can be cost-effective, or commercial systems that often come with support.
-### 3. Design Network Architecture
-- **Identify Key Areas**: Determine where to place NIDS sensors based on traffic flow, segmentation, and monitoring needs (e.g., at the perimeter, critical internal switch ports).
-- **Plan for Deployment**: Ensure that the network design accommodates the installation of NIDS, including appropriate bandwidth and security measures.
-### 4. Install and Configure NIDS
-- **Installation**: Follow the installation procedures for your chosen NIDS solution.
-- **Configuration**: Configure the system to monitor relevant network traffic, including defining rules and policies for alerting on suspicious activities. Tailor the settings to minimize false positives.
-### 5. Establish Monitoring and Alerting
-- **Set Up Alerts**: Configure alerting mechanisms so that incidents are reported to administrators or security teams in real-time.
-- **Integrate with SIEM**: Consider integrating the NIDS with a Security Information and Event Management (SIEM) system for centralized logging and advanced analysis.
-### 6. Develop Response Procedures
-- **Incident Response Plan**: Create a plan outlining how to address potential intrusions detected by the NIDS, including roles and responsibilities, investigation steps, and communication protocols.
-- **Escalation Procedures**: Define when and how to escalate incidents based on severity levels.
-### 7. Train Personnel
-- **Training Sessions**: Conduct training for your IT and security teams on how to utilize the NIDS effectively and respond to alerts.
-- **Simulated Exercises**: Regularly engage in security drills to test the effectiveness of your response procedures and the competence of your personnel.
-### 8. Continuous Monitoring and Maintenance
-- **Ongoing Monitoring**: Keep the NIDS active and continuously monitor its performance.
-- **Regular Updates**: Apply updates to the NIDS, including signature updates and system patches, to ensure it stays effective against new threats.
-- **Review and Adjust**: Periodically review policies, rules, and configurations to adapt to the changing network environment and threat landscape.
-### 9. Audit and Review
-- **Regular Audits**: Conduct regular audits of the NIDS configuration, monitoring effectiveness, and incident response performance.
-- **Reporting**: Generate reports to analyze trends, identify gaps, and support compliance requirements.
-### 10. Compliance and Documentation
-- **Document Policies and Procedures**: Ensure that all NIDS-related procedures, configurations, and policies are well documented.
-- **Compliance Check**: Make sure that your implementation aligns with relevant regulatory requirements (e.g., GDPR, PCI-DSS, HIPAA).
-By following these steps, you can effectively establish and implement a network intrusion detection system that monitors your organization's network for malicious activity, allowing you to quickly identify and address potential threats.</t>
+    <t>To implement Clause B.20.7, which requires the establishment and implementation of security policies and procedures to harden network architecture, device, and access security, follow these advanced steps:
+1. **Develop Comprehensive Security Policies**:
+   - Draft security policies that cover all aspects of network security, including device hardening, access controls, network segmentation, and incident response. Ensure these policies align with best practices and regulatory requirements (e.g., NIST, ISO 27001).
+2. **Define Hardening Guidelines**:
+   - Create detailed guidelines that specify how to harden network devices (e.g., routers, switches, firewalls). Include recommendations such as:
+     - Disabling unused ports and services.
+     - Changing default configurations and passwords.
+     - Enforcing secure management protocols (e.g., SSH instead of Telnet).
+3. **Establish Access Control Procedures**:
+   - Implement procedures for managing user access to network resources. This includes:
+     - Role-based access control (RBAC) to ensure users only have access to what they need.
+     - Regular reviews of user access permissions and revocation of access for inactive accounts.
+4. **Configuration Management**:
+   - Develop a configuration management process to track changes to network devices and ensure that all configurations are reviewed and approved before implementation. This should include maintaining baseline configurations for all devices.
+5. **Regular Security Audits and Assessments**:
+   - Schedule regular security audits to evaluate compliance with the established policies and procedures. Use vulnerability scanning tools to identify and remediate potential weaknesses in the network architecture.
+6. **Incident Response Plan**:
+   - Create an incident response plan that outlines procedures for detecting, responding to, and recovering from security incidents. Ensure that the plan includes roles, responsibilities, and communication protocols.
+7. **Training and Awareness**:
+   - Conduct training sessions for IT and security staff to ensure they understand the security policies and procedures. Foster a culture of security awareness within the organization to ensure all employees are mindful of security best practices.
+8. **Documentation and Updates**:
+   - Document all security policies, procedures, and guidelines clearly. Regularly review and update these documents to reflect changes in technology, threats, or organizational structure.
+By following these steps, you can effectively implement Clause B.20.7 and enhance your organization's network security posture through robust policies and procedures.
+What specific areas of your network architecture do you feel need the most attention regarding hardening? This will help in providing more tailored guidance.</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>Hello! It looks like you may have some questions about cybersecurity or the Cyber Trust Mark requirements from Singapore's Cyber Security Agency (CSA). If you're looking for information or guidance, please share what specific topic or question you have in mind! This will help me provide you with the best support.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.20.11?</t>
   </si>
   <si>
     <t>To implement Clause B.20.11, which requires establishing and implementing network intrusion prevention to block malicious network traffic, follow these steps:
@@ -2052,6 +2237,9 @@
 By following these steps, you can effectively establish and implement a robust network intrusion prevention strategy within your organization. Be sure to adapt these guidelines to your specific organizational environment and needs.</t>
   </si>
   <si>
+    <t>How do I implement clause B.22.2?</t>
+  </si>
+  <si>
     <t>To implement Clause B.22.2, which requires your organization to identify critical assets that need high availability and ensure there are redundancies for them, follow these step-by-step instructions:
 ### Step 1: Identify Critical Assets
 1. **Define What "Critical" Means**: Critical assets are those that are essential for your business operations. This could include:
@@ -2116,6 +2304,9 @@
 14. **Compliance Checks**: Periodically perform compliance checks and audits to ensure that the high availability strategies are being followed and that identified critical assets remain protected.
 ### Conclusion
 By following these steps, you will be able to implement a robust clause for identifying critical assets requiring high availability and ensure that appropriate redundancies are in place. Regular reviews and updates will also help maintain their effectiveness in the face of changing organizational needs.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.22.3?</t>
   </si>
   <si>
     <t>To implement Clause B.22.3, which involves conducting a business impact analysis (BIA) to identify critical processes and determine Recovery Time Objectives (RTO) and Recovery Point Objectives (RPO), follow these clear steps:
@@ -2188,6 +2379,9 @@
 2. **Update Strategies Based on Findings**: Adjust processes and plans based on the outcomes of these tests.
 ### Conclusion
 Implementing a Business Impact Analysis is a critical step in ensuring that your organization is prepared for disruptions. By defining and applying a structured BIA process, you will be better equipped to identify critical processes and establish RTOs and RPOs that align with your organization's resilience and recovery strategies.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.22.8?</t>
   </si>
   <si>
     <t>To implement Clause B.22.8, which requires establishing and implementing a policy and process to regularly test your business continuity and disaster recovery (BC/DR) plan at least once a year, follow these structured steps:
@@ -2286,6 +2480,9 @@
 By following these steps, you can effectively establish and implement a policy process to regularly test your Business Continuity and Disaster Recovery plan, ensuring it remains robust and effective in achieving its objectives.</t>
   </si>
   <si>
+    <t>How do I implement clause B.18.4?</t>
+  </si>
+  <si>
     <t>To implement Clause B.18.4, which requires your organization to perform regular vulnerability assessments at least annually, follow these beginner-friendly steps:
 ### Step 1: Understand the Requirement
 Clause B.18.4 mandates that you conduct vulnerability assessments at least once a year. These assessments should be non-intrusive, meaning they should not disrupt your systems while scanning for vulnerabilities.
@@ -2361,6 +2558,9 @@
 Here is an example of how you might word the clause for your organization’s policies:
 *"The organization shall conduct regular vulnerability assessments at least annually, utilizing non-intrusive scanning tools on all systems to identify and evaluate security vulnerabilities. Results from these assessments shall be analyzed and documented, and remediation actions will be taken to address identified vulnerabilities in a timely manner."*
 By following these steps, you can systematically implement the clause for regular vulnerability assessments within your organization, ensuring that security measures are effective and updated regularly.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.18.5?</t>
   </si>
   <si>
     <t>To implement clause B.18.5, which requires your organization to define and allocate roles and responsibilities for employees in cybersecurity vulnerability assessment and management, follow these clear steps:
@@ -2441,6 +2641,9 @@
 By defining, communicating, training, and continually evaluating roles and responsibilities related to cybersecurity vulnerability assessment and management, you can establish a robust framework that empowers employees and strengthens your organization’s cybersecurity posture. This will not only help in vulnerability management but also promote a culture of security awareness throughout the organization.</t>
   </si>
   <si>
+    <t>How do I implement clause B.18.9?</t>
+  </si>
+  <si>
     <t>To implement clause B.18.9, which requires your organization to perform regular penetration tests at least annually to discover and exploit security weaknesses, follow these steps:
 ### Step-by-Step Implementation
 1. **Understand the Importance**:
@@ -2505,6 +2708,9 @@
 - **Evidence of Testing**: Ensure that you have documented evidence to demonstrate that you meet the requirement for annual penetration testing, which could be helpful during regulatory reviews or audits.
 ### Conclusion
 By following these steps, you can effectively implement a clause for regular penetration testing in your organization. This structured approach not only fulfills the requirement but also strengthens your overall security posture against potential cyber threats.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.19.4?</t>
   </si>
   <si>
     <t>To implement clause B.19.4, which focuses on establishing physical security measures at your organization's perimeter, follow these straightforward steps:
@@ -2570,6 +2776,9 @@
 - **Continuous Improvement:** Periodically review and update security measures based on new threats and advances in security technology.
 - **Feedback Loop:** Gather feedback from employees regarding the effectiveness of security measures and make adjustments as necessary.
 By systematically implementing and maintaining these measures, an organization can significantly enhance its physical security perimeter and deter unauthorized access effectively.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.19.8?</t>
   </si>
   <si>
     <t>To implement clause B.19.8, which focuses on establishing and implementing policies and procedures for escalations and security access controls, follow these clear steps:
@@ -2644,6 +2853,9 @@
 Implementing a physical/environmental security policy and procedure is an ongoing process that requires continuous attention and adaptation to minimize impacts and maintain the integrity of the physical environment.</t>
   </si>
   <si>
+    <t>How do I implement clause B.19.11?</t>
+  </si>
+  <si>
     <t>To implement clause B.19.11, which requires establishing policies and processes for reporting physical and environmental risks to the Board and senior management, follow these structured steps:
 ### Step-by-Step Guide to Implementing Clause B.19.11
 1. **Develop Reporting Policies**:
@@ -2709,71 +2921,7 @@
 By following these steps, your organization can establish a comprehensive and effective approach to reporting physical/environmental risks that keeps the Board and senior management informed, enabling informed decision-making and proactive risk management.</t>
   </si>
   <si>
-    <t>To implement Clause B.20.4, which requires regular reviews of your network architecture and devices, follow these steps:
-### Step-by-Step Implementation of Clause B.20.4
-1. **Establish a Review Schedule**:
-   - Plan to conduct a network review at least once a year. You might want to set a specific date each year for consistency.
-2. **Create a Network Architecture Diagram**:
-   - Document your current network layout, including all devices (routers, switches, firewalls, etc.), connections, and how they interact.
-   - Tools like Microsoft Visio, Lucidchart, or even online diagramming tools can help you visualize your network.
-3. **Review Network Devices and Configurations**:
-   - Check each device’s configuration settings to ensure they comply with your security policies.
-   - Look for outdated firmware or software and update them as necessary to protect against vulnerabilities.
-4. **Identify and Remove Obsolete Rules and Protocols**:
-   - Review firewall and access control rules to ensure that they are still relevant. Remove any that are outdated or no longer necessary.
-   - Verify that protocols in use are current and secure; for instance, replace older protocols (like FTP) with secure alternatives (like SFTP).
-5. **Assign Responsibilities**:
-   - Designate a team or individual responsible for conducting these reviews. This can be a cybersecurity team or a specific IT staff member.
-   - Ensure they are trained on best practices for network security and the tools used for reviews.
-6. **Document Findings and Actions**:
-   - After each review, document any findings, updates made, and recommendations for future improvements. This record can help track changes over time and show compliance during audits.
-7. **Implement Continuous Monitoring**:
-   - Consider using network monitoring tools to continuously check for unusual activity or vulnerabilities in real-time. This can complement your annual reviews.
-### Example:
-If your network uses an old version of a routing protocol (like RIPv1), you can review this during your annual assessment and switch to a more secure version (like RIPv2) to enhance security.
-### Next Steps:
-After your review, create a checklist to streamline future assessments and ensure no crucial aspect is overlooked.
-**Question for You:**
-Do you have an existing network architecture diagram, or would you need assistance in creating one?</t>
-  </si>
-  <si>
-    <t>Implementing a clause for a network security review involves establishing a systematic process to regularly assess and update the network architecture and devices. Here is a step-by-step guide to ensure that this clause is properly implemented:
-### 1. Establish a Policy for Network Security Reviews
-- **Define Objectives:** Clearly articulate the purpose of the network security review. This could include identifying obsolete rules, ensuring compliance with standards, and safeguarding against vulnerabilities.
-- **Documentation:** Create a formal network security review policy that outlines the frequency, roles and responsibilities, processes, and standards for the review.
-### 2. Assemble a Review Team
-- **Select Members:** Form a team consisting of network security professionals, system administrators, and representatives from IT governance/risk management.
-- **Role Assignment:** Define clear roles and responsibilities for each team member to facilitate effective collaboration.
-### 3. Define the Scope of the Review
-- **Identify Assets:** Create an inventory of all network devices, including routers, switches, firewalls, and servers, as well as associated software and protocols.
-- **Review Aspects:** Decide on what to review, such as network design, access controls, firewall rules, routing protocols, and security policies.
-### 4. Develop a Review Checklist
-- **Obsolete Protocols and Rules:** Include checks for outdated rules and protocols (e.g., older versions of SSL, weak encryption methods).
-- **Configuration Management:** Ensure proper documentation of current network configurations.
-- **Risk Assessment Criteria:** Set criteria to assess the security posture of the existing network architecture.
-### 5. Schedule the Reviews
-- **Establish a Timeline:** Set an annual schedule for conducting reviews, but consider semi-annual or quarterly reviews if significant changes occur.
-- **Notifications:** Implement a notification system to remind stakeholders of upcoming reviews.
-### 6. Conduct the Review
-- **Data Collection:** Gather necessary data on network configurations, firewall and router rules, and current software versions.
-- **Analysis:** Analyze the collected data against best practices and regulatory compliance requirements.
-- **Testing:** Perform penetration testing or vulnerability assessments using tools and techniques to identify weaknesses.
-### 7. Document Findings and Recommendations
-- **Report Creation:** Compile a detailed report of findings, highlighting obsolete rules, vulnerabilities, and areas needing improvement.
-- **Recommendations:** Provide actionable recommendations for mitigating identified risks.
-### 8. Implement Changes
-- **Prioritize Actions:** Based on the severity of findings, prioritize the recommended actions for remediation.
-- **Update Configurations:** Make the necessary changes to network devices and infrastructure as per the recommendations.
-### 9. Communication and Training
-- **Stakeholder Communication:** Inform relevant stakeholders about the findings and changes made as a result of the review.
-- **Training Programs:** Conduct training sessions to ensure that IT staff and relevant personnel are up-to-date with current security policies and practices.
-### 10. Monitor and Review
-- **Continuous Monitoring:** Implement continuous monitoring tools to identify any new vulnerabilities in real time.
-- **Feedback Loop:** After changes are made, establish a feedback mechanism to evaluate the effectiveness of the newly implemented rules and configurations.
-### 11. Audit and Compliance Checks
-- **Internal Audits:** Conduct periodic internal audits to ensure compliance with the established review policy and effectiveness of the security measures.
-- **Update Policy:** Revise the network security review policy as needed based on audit results, technological changes, or evolving threats.
-By following these steps, you can effectively implement a network security review clause in your organization, ensuring that your network architecture and devices are regularly assessed and updated to mitigate potential security risks.</t>
+    <t>How do I implement clause B.20.6?</t>
   </si>
   <si>
     <t>To implement Clause B.20.6, which involves network segmentation to create separate private and public networks, follow these steps:
@@ -2849,6 +2997,33 @@
 Implementing network segmentation requires careful planning and execution but will significantly enhance your organization's security posture by protecting critical data from external threats. Regular testing and updates will ensure that the segmentation remains effective in the face of changing cybersecurity landscapes.</t>
   </si>
   <si>
+    <t>To implement Clause B.20.6, which requires the definition and application of a process for network segmentation to segregate private and public networks, follow these advanced steps:
+1. **Define Network Segmentation Strategy**:
+   - Establish a clear strategy for how your organization will segment its networks into private and public segments. Ensure that the private network is dedicated to business-critical data and has no direct connection to the Internet.
+2. **Design the Network Architecture**:
+   - Create a detailed network diagram that illustrates the segmentation, highlighting which devices and data reside in the private network versus the public network. Ensure that business-critical systems are isolated within the private segment.
+3. **Utilize Virtual Private Cloud (VPC) Solutions**:
+   - If using cloud infrastructure (e.g., AWS, Azure), leverage their VPC capabilities to create isolated environments. For instance:
+     - **AWS VPC**: Set up a VPC with public and private subnets. Ensure that the private subnets do not have Internet access.
+     - **Azure VNet**: Use Azure Virtual Network to define subnets and apply Network Security Groups (NSGs) to control traffic.
+4. **Implement Network Access Control Lists (ACLs)**:
+   - Configure ACLs to control inbound and outbound traffic between the public and private segments. Define rules that only allow necessary communication while denying all other traffic.
+   - Example: Allow HTTP/HTTPS traffic from public to a web server in the public subnet, while restricting access from the public subnet to the private subnet.
+5. **Deploy Security Groups**:
+   - Utilize security groups to apply additional layers of security. Configure security group rules for resources within the private network to restrict access to only trusted IP addresses or services.
+6. **No Direct Internet Connection for Private Network**:
+   - Ensure that the private network segment is configured without a direct Internet connection. If access is required (for software updates, etc.), implement a controlled method such as a jump box or bastion host that allows monitored and logged access.
+7. **Regular Audits and Monitoring**:
+   - Conduct regular audits of the network segmentation setup to ensure compliance with the defined policies. Use monitoring tools to track traffic flows and detect any unauthorized access attempts between segments.
+8. **Document and Train**:
+   - Document the network segmentation process, including diagrams, policies, and configurations. Train IT staff on maintaining the segmentation and responding to potential security incidents.
+By following these steps, you can effectively implement Clause B.20.6 and enhance your organization’s security posture through proper network segmentation.
+What specific technologies or cloud platforms are you currently using for your network infrastructure? This will help tailor the recommendations further.</t>
+  </si>
+  <si>
+    <t>How do I implement clause B.20.10?</t>
+  </si>
+  <si>
     <t>To implement Clause B.20.10, which involves establishing and implementing policies and processes to evaluate the performance of network security devices, follow these steps:
 ### Step-by-Step Implementation of Clause B.20.10
 1. **Define Evaluation Objectives**:
@@ -2921,121 +3096,95 @@
 By following these steps, your organization will establish and implement a structured approach towards evaluating and continuously improving the performance of network security devices. This not only helps in blocking malicious traffic more effectively but also strengthens the overall cyber defense posture of the organization.</t>
   </si>
   <si>
-    <t>Identifying assets requiring high availability: Has the organisation identified the critical assets in the organisation that require high availability and performed measures to ensure that there are redundancies for them?</t>
-  </si>
-  <si>
-    <t>Business impact analysis: Has the organisation defined and applied the process of business impact analysis to identify the critical processes and expected RTO and RPO for business resumption?</t>
-  </si>
-  <si>
-    <t>Redundancy process: Has the organisation defined and applied the process to perform redundancy on systems to ensure the cyber resilience of its systems?</t>
-  </si>
-  <si>
-    <t>Business continuity/disaster recovery policy: Has the organisation established and implemented the business continuity/disaster recovery policies with the requirements, roles and responsibilities and guidelines including the RTO and RPO to ensure that business resumption can be carried out in accordance with the system's criticality?</t>
-  </si>
-  <si>
-    <t>Business continuity/disaster recovery plan: Has the organisation established and implemented a business continuity/disaster recovery plan to respond and recover against the common business disruption scenarios including those caused by cybersecurity incidents to ensure cyber resiliency.</t>
-  </si>
-  <si>
-    <t>Business continuity/disaster recovery plan review: Does the organisation perform regular reviews at least on an annual basis on the business continuity/disaster recovery plan to ensure that it is kept up to date?</t>
-  </si>
-  <si>
-    <t>Business continuity/disaster recovery plan test: Has the organisation established and implemented the policy process to test on its business continuity/disaster recovery plan regularly at least on an annual basis to ensure the effectiveness of the plan in achieving its objectives?</t>
-  </si>
-  <si>
-    <t>Monitoring against RTO/RPO: Does the organisation perform monitoring on the RTO and RPO during business continuity/disaster recovery to ensure that it falls within the targets and report the findings to the Board and/or senior management?</t>
-  </si>
-  <si>
-    <t>Business continuity/disaster recovery exercise: Does the organisation perform coordinated business continuity/disaster recovery exercise with its third parties for an extended period of time to evaluate the effectiveness of the processes and procedures?</t>
-  </si>
-  <si>
-    <t>Access control to the network: Has the organisation configured and implemented access control (e.g., whitelisting, blacklisting) to its network to enforce network security policy and ensure that unauthorised users and/or devices are kept out?</t>
-  </si>
-  <si>
-    <t>Stateful firewall: Has the organisation established and implemented the use of stateful firewall over basic packet filtering firewall to ensure yjay packets are filtered with more context for greater effectiveness?</t>
-  </si>
-  <si>
-    <t>Network security review: Have the network architecture and devices been reviewed regularly at least on an annual basis to ensure yjay they are up to date without obsolete rules and protocols?</t>
-  </si>
-  <si>
-    <t>Network security process: Has the organisation defined and implemented the process to configure both wired and wireless networks securely, minimally with the use of secure network authentication and encryption protocol and disabling Wi-Fi Protected Setup (WPS) to ensure that the network is secured and data is not lost or breached through the network?</t>
-  </si>
-  <si>
-    <t>Network segmentation: Has the organisation defined and applied a process to carry out network segmentation to segregate into private and public networks with the private network holding all the business-critical data and having no connection to the Internet to ensure that it is isolated from external threats?</t>
-  </si>
-  <si>
-    <t>Network security policies and procedures: Has the organisation established and implemented security policies and procedures with the requirements, guidelines and detailed steps to harden the network architecture, device and access security?</t>
-  </si>
-  <si>
-    <t>Roles and responsibilities: Has the organisation defined and allocated roles and responsibilities to oversee, manage and monitor network security to ensure that the employees are clear of the tasks assigned to them?</t>
-  </si>
-  <si>
-    <t>Network Intrusion Detection: Has the organisation established and implemented network intrusion detection on the organisation's network to monitor and detect malicious network traffic to ensure that they can be identified and addressed in a timely manner?</t>
-  </si>
-  <si>
-    <t>Improvement on network security devices: Has the organisation established and implemented the policies and processes to evaluate the performance of the network security devices in term of its effectiveness in blocking malicious traffic and carrying out improvements?</t>
-  </si>
-  <si>
-    <t>Network Intrusion Prevention: Has the organisation established and implemented network intrusion prevention on the organisation's network to block malicious network traffic and ensure that it is protected from threats?</t>
-  </si>
-  <si>
-    <t>Detective control: Has the organisation identified the physical/environmental risks in its environment and implemented detective measures to be alerted on threats to ensure that they are addressed in a timely manner?</t>
-  </si>
-  <si>
-    <t>Protection against internal and external threats: Does the organisation perform measures to protect its physical assets against internal and external threats, e.g., the use of cable lock to ensure that they are not stolen or tampered with?</t>
-  </si>
-  <si>
-    <t>Security perimeter: Has the organisation implemented physical security measures on its perimeter, e.g., fence and gate to deter unauthorised access into the premises of the organisation?</t>
-  </si>
-  <si>
-    <t>Preventive process: Has the organisation defined and implemented the process to ensure that visitors are registered and authorised before having access to the premises of the organisation?</t>
-  </si>
-  <si>
-    <t>Monitoring process: Has the organisation defined and implemented the process to monitor its premises on a 24/7 basis, e.g., through the use of CCTV to deter and investigate on any physical/environmental threats?</t>
-  </si>
-  <si>
-    <t>Physical media handling process: Has the organisation defined and applied the process to store and transport physical media containing business-critical data securely within and out of the premise to ensure confidential and/or sensitive are protected?</t>
-  </si>
-  <si>
-    <t>Physical/environmental security policy and procedure: Has the organisation established and implemented the policies and procedures with the requirements, guidelines and detailed steps for escalations security access controls to minimise the impact and interference to its physical environment?</t>
-  </si>
-  <si>
-    <t>Roles and responsibilities: Has the organisation defined and allocated the roles and responsibilities in detecting, mitigating and responding against physical/environmental risks to ensure yjay employees are clear of the tasks assigned to them?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physical/environment review: Has the organisation established and implemented the policies and procedures on the requirements, guidelines and detailed steps to perform reviews on the physical security measures and assets to ensure that they remain secure? </t>
-  </si>
-  <si>
-    <t>Reporting of physical/environmental risks: Has the organisation established and implemented policies and processes to report physical/environmental risk and controls to the Board and/or senior managed to ensure that they are kept informed of the risks?</t>
-  </si>
-  <si>
-    <t>Improvement on physical/environmental controls: Has the organisation established and implemented a process to review and improve the physical/environmental security measures to ensure that they are effective?</t>
-  </si>
-  <si>
-    <t>Vulnerability assessment plan: Has the organisation established a vulnerability assessment plan with objectives, scope and requirements to review and perform vulnerability assessment on its systems?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vulnerability assessment: Does the organisation perform regular vulnerability assessment at least on an annual basis to perform non-intrusive scans on its systems to ensure that vulnerabilities are discovered? </t>
-  </si>
-  <si>
-    <t>Roles and responsibilities: Has the organisation defined and allocated roles and responsibilities for its employees on carrying out cybersecurity vulnerability assessment and management?</t>
-  </si>
-  <si>
-    <t>Vulnerability assessment policy and procedure: Has the organisation established and implemented policies and procedures on the requirements, guidelines and detailed steps for conducting cybersecurity vulnerability assessments across its systems to ensure that steps are taken to address the associated risk vulnerabilities identified in a timely manner.</t>
-  </si>
-  <si>
-    <t>Tracking and remediating identified vulnerabilities: Has the organisation established and implemented measures and processes to track, review, evaluate and address the vulnerabilities uncovered as part of the assessments to ensure that the vulnerabilities are being remediated according to their severity?</t>
-  </si>
-  <si>
-    <t>Penetration test plan: Has the organisation established and implemented a penetration test plan with the objectives, scope, rules of engagement to ensure that the penetration test can be performed safely?</t>
-  </si>
-  <si>
-    <t>Penetration testing: Does the organisation perform a regular penetration test at least on an annual basis to discover and exploit security weakness(es) in its systems to ensure that its system's security can be evaluated?</t>
-  </si>
-  <si>
-    <t>Follow up on vulnerability assessment findings: Has the organisation established and implemented metrics and thresholds including dashboards to provide reporting and tracking of open, overdue and severe vulnerabilities noted within its systems in order to provide visibility on tracking and remediations within established timelines?</t>
-  </si>
-  <si>
-    <t>Reporting of vulnerability assessment result: Has the organisation established and implemented practices and measures to regularly report on the vulnerability assessment results and findings to the Board and/or senior management?</t>
+    <t>How do I implement clause B.20.4?</t>
+  </si>
+  <si>
+    <t>To implement Clause B.20.4, which requires regular reviews of your network architecture and devices, follow these steps:
+### Step-by-Step Implementation of Clause B.20.4
+1. **Establish a Review Schedule**:
+   - Plan to conduct a network review at least once a year. You might want to set a specific date each year for consistency.
+2. **Create a Network Architecture Diagram**:
+   - Document your current network layout, including all devices (routers, switches, firewalls, etc.), connections, and how they interact.
+   - Tools like Microsoft Visio, Lucidchart, or even online diagramming tools can help you visualize your network.
+3. **Review Network Devices and Configurations**:
+   - Check each device’s configuration settings to ensure they comply with your security policies.
+   - Look for outdated firmware or software and update them as necessary to protect against vulnerabilities.
+4. **Identify and Remove Obsolete Rules and Protocols**:
+   - Review firewall and access control rules to ensure that they are still relevant. Remove any that are outdated or no longer necessary.
+   - Verify that protocols in use are current and secure; for instance, replace older protocols (like FTP) with secure alternatives (like SFTP).
+5. **Assign Responsibilities**:
+   - Designate a team or individual responsible for conducting these reviews. This can be a cybersecurity team or a specific IT staff member.
+   - Ensure they are trained on best practices for network security and the tools used for reviews.
+6. **Document Findings and Actions**:
+   - After each review, document any findings, updates made, and recommendations for future improvements. This record can help track changes over time and show compliance during audits.
+7. **Implement Continuous Monitoring**:
+   - Consider using network monitoring tools to continuously check for unusual activity or vulnerabilities in real-time. This can complement your annual reviews.
+### Example:
+If your network uses an old version of a routing protocol (like RIPv1), you can review this during your annual assessment and switch to a more secure version (like RIPv2) to enhance security.
+### Next Steps:
+After your review, create a checklist to streamline future assessments and ensure no crucial aspect is overlooked.
+**Question for You:**
+Do you have an existing network architecture diagram, or would you need assistance in creating one?</t>
+  </si>
+  <si>
+    <t>Implementing a clause for a network security review involves establishing a systematic process to regularly assess and update the network architecture and devices. Here is a step-by-step guide to ensure that this clause is properly implemented:
+### 1. Establish a Policy for Network Security Reviews
+- **Define Objectives:** Clearly articulate the purpose of the network security review. This could include identifying obsolete rules, ensuring compliance with standards, and safeguarding against vulnerabilities.
+- **Documentation:** Create a formal network security review policy that outlines the frequency, roles and responsibilities, processes, and standards for the review.
+### 2. Assemble a Review Team
+- **Select Members:** Form a team consisting of network security professionals, system administrators, and representatives from IT governance/risk management.
+- **Role Assignment:** Define clear roles and responsibilities for each team member to facilitate effective collaboration.
+### 3. Define the Scope of the Review
+- **Identify Assets:** Create an inventory of all network devices, including routers, switches, firewalls, and servers, as well as associated software and protocols.
+- **Review Aspects:** Decide on what to review, such as network design, access controls, firewall rules, routing protocols, and security policies.
+### 4. Develop a Review Checklist
+- **Obsolete Protocols and Rules:** Include checks for outdated rules and protocols (e.g., older versions of SSL, weak encryption methods).
+- **Configuration Management:** Ensure proper documentation of current network configurations.
+- **Risk Assessment Criteria:** Set criteria to assess the security posture of the existing network architecture.
+### 5. Schedule the Reviews
+- **Establish a Timeline:** Set an annual schedule for conducting reviews, but consider semi-annual or quarterly reviews if significant changes occur.
+- **Notifications:** Implement a notification system to remind stakeholders of upcoming reviews.
+### 6. Conduct the Review
+- **Data Collection:** Gather necessary data on network configurations, firewall and router rules, and current software versions.
+- **Analysis:** Analyze the collected data against best practices and regulatory compliance requirements.
+- **Testing:** Perform penetration testing or vulnerability assessments using tools and techniques to identify weaknesses.
+### 7. Document Findings and Recommendations
+- **Report Creation:** Compile a detailed report of findings, highlighting obsolete rules, vulnerabilities, and areas needing improvement.
+- **Recommendations:** Provide actionable recommendations for mitigating identified risks.
+### 8. Implement Changes
+- **Prioritize Actions:** Based on the severity of findings, prioritize the recommended actions for remediation.
+- **Update Configurations:** Make the necessary changes to network devices and infrastructure as per the recommendations.
+### 9. Communication and Training
+- **Stakeholder Communication:** Inform relevant stakeholders about the findings and changes made as a result of the review.
+- **Training Programs:** Conduct training sessions to ensure that IT staff and relevant personnel are up-to-date with current security policies and practices.
+### 10. Monitor and Review
+- **Continuous Monitoring:** Implement continuous monitoring tools to identify any new vulnerabilities in real time.
+- **Feedback Loop:** After changes are made, establish a feedback mechanism to evaluate the effectiveness of the newly implemented rules and configurations.
+### 11. Audit and Compliance Checks
+- **Internal Audits:** Conduct periodic internal audits to ensure compliance with the established review policy and effectiveness of the security measures.
+- **Update Policy:** Revise the network security review policy as needed based on audit results, technological changes, or evolving threats.
+By following these steps, you can effectively implement a network security review clause in your organization, ensuring that your network architecture and devices are regularly assessed and updated to mitigate potential security risks.</t>
+  </si>
+  <si>
+    <t>To implement Clause B.20.4, which requires the regular review of network architecture and devices at least annually to ensure they are up to date and free from obsolete rules and protocols, follow these advanced steps:
+1. **Establish a Review Schedule**:
+   - Create a calendar to ensure that network architecture reviews occur at least once a year. This schedule should include specific dates and responsible personnel.
+2. **Document Current Network Architecture**:
+   - Maintain an up-to-date network architecture diagram that includes all devices, connections, and protocols in use. This documentation is crucial for identifying obsolete components.
+3. **Conduct a Comprehensive Review**:
+   - **Review Network Devices**: Examine all network devices (routers, switches, firewalls, etc.) to ensure they are running the latest firmware and software versions. Identify any devices that may be outdated or nearing end-of-life.
+   - **Evaluate Security Policies**: Review existing network security policies and configurations. Ensure that they align with current organizational needs and do not include obsolete rules or protocols.
+   - **Assess Protocol Usage**: Identify protocols that are no longer deemed secure (e.g., deprecated versions of SSL/TLS) and replace them with up-to-date alternatives.
+4. **Utilize Compliance Tools**:
+   - Implement network management or compliance tools that can automatically audit your network architecture against industry standards (e.g., NIST, ISO 27001) to identify non-compliance or outdated configurations.
+5. **Engage the Cybersecurity Team**:
+   - Ensure that the cybersecurity team is involved in the review process. They should track changes, confirm compliance, and provide insights on emerging threats that may impact the network architecture.
+6. **Document Findings and Actions**:
+   - After the review, document the findings, including any obsolete rules or protocols that were identified and the actions taken to address them. This documentation should also include a plan for remediation and timelines for implementing changes.
+7. **Training and Awareness**:
+   - Provide training sessions for relevant staff on the importance of maintaining an updated network architecture and how to recognize and mitigate risks associated with obsolete components.
+By following these steps, you can ensure that your network architecture remains current and secure, thereby fulfilling the requirements of Clause B.20.4.
+What specific tools or processes do you currently use for managing your network architecture? This will help tailor further recommendations.</t>
   </si>
 </sst>
 </file>
@@ -3052,7 +3201,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3060,7 +3209,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3110,20 +3259,6 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3135,9 +3270,8 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
+        <color rgb="FFFF0000"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3150,6 +3284,20 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
       </border>
     </dxf>
   </dxfs>
@@ -3165,25 +3313,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE4BEF0F-BDB0-45A9-A2CA-5C3F58EB0DD8}" name="Table1" displayName="Table1" ref="A1:H40" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:H40" xr:uid="{AE4BEF0F-BDB0-45A9-A2CA-5C3F58EB0DD8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H40">
-    <sortCondition ref="C1:C40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4869336B-2055-4A66-8B07-FC69451D4720}" name="Table1" displayName="Table1" ref="A1:J41" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:J41" xr:uid="{4869336B-2055-4A66-8B07-FC69451D4720}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J41">
+    <sortCondition ref="B1:B41"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{AE7DC592-77F1-4469-BCCE-0EC915E9A3B9}" name="id"/>
-    <tableColumn id="2" xr3:uid="{C6162709-7325-4881-AC3E-EC82B8D81CE5}" name="question"/>
-    <tableColumn id="3" xr3:uid="{A0F0787A-E21C-42F1-B3AD-6443FF71A577}" name="my_answer"/>
-    <tableColumn id="4" xr3:uid="{70E76444-1ED8-4C4E-9C42-2A28FA49DA14}" name="my_grade"/>
-    <tableColumn id="5" xr3:uid="{25A9E98E-42D7-4851-A210-DCA1E919E5BE}" name="gpt_answer"/>
-    <tableColumn id="6" xr3:uid="{2E4BC64E-2D73-4959-BD24-96577FBE24CE}" name="gpt_grade"/>
-    <tableColumn id="7" xr3:uid="{7D735A39-27B5-4B2E-8684-308B5E860809}" name="reason"/>
-    <tableColumn id="8" xr3:uid="{DE12FB92-C69B-46C8-BA12-9ECAD80AB715}" name="better_answer"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{F4B74CB5-15BE-4446-A4B3-719F157638E9}" name="id"/>
+    <tableColumn id="2" xr3:uid="{CECB8EE2-E03A-40F1-84FE-D28EE9BB05BA}" name="question"/>
+    <tableColumn id="3" xr3:uid="{ADD35783-8A03-4408-98AF-9B71B81951B8}" name="my_answer"/>
+    <tableColumn id="4" xr3:uid="{B8362A23-1AAD-4D5B-AE64-2BA0BFD393A3}" name="my_grade"/>
+    <tableColumn id="5" xr3:uid="{83130CB8-3419-4C76-8D9A-792F78346F32}" name="gpt_answer"/>
+    <tableColumn id="6" xr3:uid="{3D18C911-5BD4-4FA9-8720-D2E78F0DD59E}" name="gpt_grade"/>
+    <tableColumn id="7" xr3:uid="{FEA76A36-5925-40F7-BF74-B395139D43A2}" name="reason"/>
+    <tableColumn id="8" xr3:uid="{59C68915-DA8F-45DE-BDE0-302798C064CE}" name="better_answer"/>
+    <tableColumn id="9" xr3:uid="{CF6EDE9B-5FCB-4309-A31F-45B0C8A2D7AF}" name="advanced_answer"/>
+    <tableColumn id="10" xr3:uid="{9600F015-177C-4C6F-9F21-473CA42AF792}" name="better_advanced_answer"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3474,23 +3620,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3515,551 +3663,586 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" t="s">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" t="s">
+        <v>133</v>
+      </c>
+      <c r="I27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
         <v>124</v>
       </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>69</v>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="B32" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>32</v>
-      </c>
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>38</v>
-      </c>
-      <c r="B30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>94</v>
-      </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E34" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>10</v>
       </c>
-      <c r="B40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" t="s">
-        <v>19</v>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>